<commit_message>
Update encyclopedia script and table
</commit_message>
<xml_diff>
--- a/encyclopedia/encyclopedia_table.xlsx
+++ b/encyclopedia/encyclopedia_table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="563">
   <si>
     <t>High-hierarchy cell types</t>
   </si>
@@ -127,7 +127,7 @@
     <t>pDC precursor</t>
   </si>
   <si>
-    <t>Plasmablasts</t>
+    <t>Plasma cells</t>
   </si>
   <si>
     <t>Promyelocytes</t>
@@ -238,6 +238,12 @@
     <t>ILC3</t>
   </si>
   <si>
+    <t>CD16+ NK cells</t>
+  </si>
+  <si>
+    <t>CD16- NK cells</t>
+  </si>
+  <si>
     <t>NK cells</t>
   </si>
   <si>
@@ -253,6 +259,12 @@
     <t>Kupffer cells</t>
   </si>
   <si>
+    <t>Classical monocytes</t>
+  </si>
+  <si>
+    <t>Non-classical monocytes</t>
+  </si>
+  <si>
     <t>CD8a/a</t>
   </si>
   <si>
@@ -454,6 +466,12 @@
     <t>innate lymphoid cell subpopulation III that is required for host defense against specific extracellular bacteria and fungi</t>
   </si>
   <si>
+    <t>CD16+ granular lymphocytes that play protective roles against both infectious pathogens and cancer using antibody-dependent cell-mediated cytotoxicity</t>
+  </si>
+  <si>
+    <t>CD16- granular lymphocytes that play protective roles against both infectious pathogens and cancer using antibody-dependent cell-mediated cytotoxicity</t>
+  </si>
+  <si>
     <t>granular lymphocytes that play protective roles against both infectious pathogens and cancer using antibody-dependent cell-mediated cytotoxicity</t>
   </si>
   <si>
@@ -493,6 +511,12 @@
     <t>monocyte precursors that are committed to the monocytes</t>
   </si>
   <si>
+    <t>CD14+ myeloid mononuclear recirculating leukocytes that are capable of differentiating into macrophages and myeloid lineage dendritic cells</t>
+  </si>
+  <si>
+    <t>CD16+ myeloid mononuclear recirculating leukocytes that are capable of differentiating into macrophages and myeloid lineage dendritic cells</t>
+  </si>
+  <si>
     <t>myeloid mononuclear recirculating leukocytes that are capable of differentiating into macrophages and myeloid lineage dendritic cells</t>
   </si>
   <si>
@@ -505,7 +529,7 @@
     <t>precursors of plasmacytoid dendritic cells which have intermixed lymphoid and myeloid origins and give rise to plasmacytoid dendritic cells</t>
   </si>
   <si>
-    <t>rapidly dividing and short-lived antibody-secreting plasma cells between post germinal centre B cells and mature plasma cells</t>
+    <t>B-lymphocyte white blood cells capable of secreting large quantities of immunoglobulins or antibodies</t>
   </si>
   <si>
     <t>early granulocyte progenitors in the bone marrow which are derived from the myeloblasts and develop into the myelocytes</t>
@@ -715,6 +739,12 @@
     <t>CL:0000113</t>
   </si>
   <si>
+    <t>CL:0000860</t>
+  </si>
+  <si>
+    <t>CL:0000875</t>
+  </si>
+  <si>
     <t>CL:0002193</t>
   </si>
   <si>
@@ -769,292 +799,379 @@
     <t>CL:0000899</t>
   </si>
   <si>
-    <t>Blood, Eye, Intestine, Kidney, Liver, Lung, Trachea, Upper airway</t>
+    <t>Blood, Colon, Decidua, Eye, Intestine, Kidney, Liver, Lung, Spleen, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Colon, Omentum adipose tissue</t>
+  </si>
+  <si>
+    <t>Colon, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Kidney, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Liver</t>
+  </si>
+  <si>
+    <t>Liver, Thymus</t>
+  </si>
+  <si>
+    <t>Colon</t>
+  </si>
+  <si>
+    <t>Spleen</t>
+  </si>
+  <si>
+    <t>Colon, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Kidney, Lung, Oesophagus, Omentum adipose tissue, Upper airway</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Liver, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Liver, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Liver, Omentum adipose tissue</t>
+  </si>
+  <si>
+    <t>Thymus</t>
+  </si>
+  <si>
+    <t>Omentum adipose tissue, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Thymus</t>
+  </si>
+  <si>
+    <t>Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Thymus, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Liver</t>
+  </si>
+  <si>
+    <t>Blood, Decidua</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Kidney, Omentum adipose tissue, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Intestine, Liver</t>
+  </si>
+  <si>
+    <t>Bone marrow</t>
+  </si>
+  <si>
+    <t>Liver</t>
+  </si>
+  <si>
+    <t>Blood, Colon, Intestine, Mesenteric lymph node, Oesophagus, Spleen</t>
+  </si>
+  <si>
+    <t>Omentum adipose tissue, Tonsil</t>
+  </si>
+  <si>
+    <t>Blood, Tonsil</t>
+  </si>
+  <si>
+    <t>Blood, Decidua, Omentum adipose tissue, Thymus, Tonsil</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Liver, Lung, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus, Tonsil</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Liver, Lung, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Tonsil, Trachea</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Omentum adipose tissue</t>
+  </si>
+  <si>
+    <t>Decidua, Placenta</t>
+  </si>
+  <si>
+    <t>Kidney</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Eye, Intestine, Lung, Mesenteric lymph node, Omentum adipose tissue, Placenta, Spleen, Thymus, Trachea, Upper airway</t>
+  </si>
+  <si>
+    <t>Bone marrow, Colon, Eye, Intestine, Liver, Lung, Oesophagus, Thymus</t>
+  </si>
+  <si>
+    <t>Intestine, Omentum adipose tissue</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Liver, Oesophagus, Omentum adipose tissue, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Kidney, Liver, Lung, Omentum adipose tissue, Spleen, Thymus, Upper airway</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Liver, Lung, Omentum adipose tissue, Spleen, Thymus, Upper airway</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Decidua, Kidney, Lung, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Intestine, Lung, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen, Thymus, Upper airway</t>
+  </si>
+  <si>
+    <t>Colon, Mesenteric lymph node, Spleen, Thymus</t>
   </si>
   <si>
     <t>Colon, Mesenteric lymph node</t>
   </si>
   <si>
-    <t>Colon, Spleen</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Mesenteric lymph node, Oesophagus, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Oesophagus, Omentum adipose tissue, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Bone marrow</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow</t>
-  </si>
-  <si>
-    <t>Bone marrow, Liver</t>
-  </si>
-  <si>
-    <t>Liver, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Liver</t>
-  </si>
-  <si>
-    <t>Colon</t>
-  </si>
-  <si>
-    <t>Spleen</t>
-  </si>
-  <si>
-    <t>Blood, Kidney, Lung, Oesophagus, Upper airway</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Liver, Mesenteric lymph node, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Liver, Mesenteric lymph node, Placenta, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Thymus</t>
-  </si>
-  <si>
-    <t>Thymus, Trachea</t>
-  </si>
-  <si>
-    <t>Blood, Liver</t>
-  </si>
-  <si>
-    <t>Blood, Decidua, Placenta</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Kidney, Spleen</t>
-  </si>
-  <si>
-    <t>Liver</t>
-  </si>
-  <si>
-    <t>Colon, Intestine, Mesenteric lymph node, Spleen</t>
-  </si>
-  <si>
-    <t>Tonsil</t>
-  </si>
-  <si>
-    <t>Decidua, Thymus, Tonsil</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Liver, Lung, Mesenteric lymph node, Omentum adipose tissue, Placenta, Spleen, Thymus, Tonsil, Trachea, Upper airway</t>
-  </si>
-  <si>
-    <t>Decidua</t>
-  </si>
-  <si>
-    <t>Kidney</t>
-  </si>
-  <si>
-    <t>Colon, Decidua, Eye, Intestine, Kidney, Liver, Lung, Mesenteric lymph node, Omentum adipose tissue, Placenta, Spleen, Thymus, Trachea, Upper airway</t>
-  </si>
-  <si>
-    <t>Colon, Eye, Intestine, Liver, Lung, Oesophagus, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Liver, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Intestine</t>
-  </si>
-  <si>
-    <t>Bone marrow, Liver, Oesophagus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Liver, Lung, Mesenteric lymph node, Omentum adipose tissue, Placenta, Spleen, Thymus, Upper airway</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Kidney, Mesenteric lymph node, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Mesenteric lymph node, Placenta, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Spleen</t>
-  </si>
-  <si>
-    <t>Colon, Mesenteric lymph node, Spleen, Thymus</t>
-  </si>
-  <si>
-    <t>Colon, Mesenteric lymph node, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Skin, Spleen</t>
-  </si>
-  <si>
-    <t>Blood, Decidua</t>
-  </si>
-  <si>
-    <t>Kidney, Thymus</t>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Kidney, Lung, Lung-draining lymph node, Mesenteric lymph node, Oesophagus, Omentum adipose tissue, Skin, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Decidua, Spleen</t>
+  </si>
+  <si>
+    <t>Blood, Kidney, Thymus</t>
   </si>
   <si>
     <t>Blood, Bone marrow, Colon, Decidua, Intestine, Mesenteric lymph node, Skin, Spleen, Thymus</t>
   </si>
   <si>
-    <t>Intestine, Lung, Spleen, Trachea, Upper airway</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Decidua, Thymus</t>
-  </si>
-  <si>
-    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Mesenteric lymph node, Omentum adipose tissue, Thymus</t>
-  </si>
-  <si>
-    <t>Eye, Oesophagus, Spleen, Thymus</t>
+    <t>Blood, Bone marrow, Eye, Intestine, Kidney, Lung, Omentum adipose tissue, Spleen, Thymus, Trachea, Upper airway</t>
+  </si>
+  <si>
+    <t>Blood, Intestine, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Decidua, Mesenteric lymph node, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Bone marrow, Colon, Decidua, Intestine, Mesenteric lymph node, Omentum adipose tissue, Spleen, Thymus</t>
+  </si>
+  <si>
+    <t>Blood, Eye, Kidney, Spleen, Thymus</t>
   </si>
   <si>
     <t>Blood, Bone marrow, Omentum adipose tissue, Thymus</t>
   </si>
   <si>
-    <t>Braga et al. 2019, Martin et al. 2019, Miller et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Voigt et al. 2019, Zheng et al. 2017</t>
+    <t>Blood, Omentum adipose tissue, Thymus</t>
+  </si>
+  <si>
+    <t>Bone marrow, Colon, Mesenteric lymph node, Omentum adipose tissue</t>
+  </si>
+  <si>
+    <t>Blood, Colon, Intestine, Mesenteric lymph node, Thymus</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Voigt et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Stewart et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Popescu et al. 2019</t>
+  </si>
+  <si>
+    <t>Park et al. 2020, Popescu et al. 2019</t>
   </si>
   <si>
     <t>James et al. 2020, Smillie et al. 2019</t>
   </si>
   <si>
+    <t>James et al. 2020</t>
+  </si>
+  <si>
+    <t>Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>Madissoon et al. 2020</t>
+  </si>
+  <si>
     <t>Madissoon et al. 2020, Smillie et al. 2019</t>
   </si>
   <si>
-    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Popescu et al. 2019</t>
-  </si>
-  <si>
-    <t>Park et al. 2020, Popescu et al. 2019</t>
-  </si>
-  <si>
-    <t>James et al. 2020</t>
-  </si>
-  <si>
-    <t>Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>Madissoon et al. 2020</t>
-  </si>
-  <si>
-    <t>Braga et al. 2019, Madissoon et al. 2020, Stewart et al. 2019, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Vento-Tormo et al. 2018</t>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Stewart et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Vento-Tormo et al. 2018</t>
   </si>
   <si>
     <t>Madissoon et al. 2020, Park et al. 2020</t>
   </si>
   <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Popescu et al. 2019</t>
+  </si>
+  <si>
     <t>Park et al. 2020</t>
   </si>
   <si>
+    <t>Jaitin et al. 2019, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>Park et al. 2020, Zheng et al. 2017</t>
+  </si>
+  <si>
     <t>Miller et al. 2020, Park et al. 2020</t>
   </si>
   <si>
+    <t>Miller et al. 2020, Park et al. 2020, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Popescu et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
     <t>Vento-Tormo et al. 2018</t>
   </si>
   <si>
-    <t>HCA Immune 2018, Madissoon et al. 2020, Stewart et al. 2019</t>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Stewart et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Li et al. 2019, Popescu et al. 2019</t>
   </si>
   <si>
     <t>Popescu et al. 2019</t>
   </si>
   <si>
-    <t>James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Smillie et al. 2019</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016, Park et al. 2020, Vento-Tormo et al. 2018</t>
-  </si>
-  <si>
-    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Smillie et al. 2019</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Jaitin et al. 2019</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Jaitin et al. 2019, Park et al. 2020, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Bjorklund et al. 2016, Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019</t>
   </si>
   <si>
     <t>Stewart et al. 2019</t>
   </si>
   <si>
-    <t>Braga et al. 2019, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Miller et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Voigt et al. 2019</t>
-  </si>
-  <si>
-    <t>Braga et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Voigt et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019</t>
-  </si>
-  <si>
-    <t>Martin et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Madissoon et al. 2020, Popescu et al. 2019</t>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Miller et al. 2020, Park et al. 2020, Smillie et al. 2019, Vento-Tormo et al. 2018, Voigt et al. 2019</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Voigt et al. 2019</t>
+  </si>
+  <si>
+    <t>Jaitin et al. 2019, Martin et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
     <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Popescu et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
-    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Stewart et al. 2019</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Smillie et al. 2019, Vento-Tormo et al. 2018</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
+    <t>Braga et al. 2019, HCA Immune 2018, Madissoon et al. 2020, Park et al. 2020, Stewart et al. 2019, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Martin et al. 2019, Park et al. 2020, Smillie et al. 2019, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Madissoon et al. 2020, Park et al. 2020, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
     <t>James et al. 2020, Madissoon et al. 2020, Park et al. 2020</t>
   </si>
   <si>
-    <t>James et al. 2020, Park et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Madissoon et al. 2020, Miragaia et al. 2019, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Park et al. 2020, Stewart et al. 2019</t>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miragaia et al. 2019, Park et al. 2020, Smillie et al. 2019, Stewart et al. 2019, Szabo et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Madissoon et al. 2020, Vento-Tormo et al. 2018</t>
+  </si>
+  <si>
+    <t>Park et al. 2020, Stewart et al. 2019, Zheng et al. 2017</t>
   </si>
   <si>
     <t>HCA Immune 2018, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Miragaia et al. 2019, Park et al. 2020, Smillie et al. 2019, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
   </si>
   <si>
-    <t>Braga et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Park et al. 2020, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Park et al. 2020, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
-  </si>
-  <si>
-    <t>Madissoon et al. 2020, Park et al. 2020, Voigt et al. 2019</t>
+    <t>Braga et al. 2019, HCA Immune 2018, Jaitin et al. 2019, Li et al. 2019, Madissoon et al. 2020, Martin et al. 2019, Miller et al. 2020, Park et al. 2020, Stewart et al. 2019, Voigt et al. 2019</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Li et al. 2019, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Madissoon et al. 2020, Park et al. 2020, Vento-Tormo et al. 2018, Zhang et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020, Li et al. 2019, Madissoon et al. 2020, Park et al. 2020, Vento-Tormo et al. 2018, Zheng et al. 2017</t>
+  </si>
+  <si>
+    <t>Madissoon et al. 2020, Park et al. 2020, Stewart et al. 2019, Voigt et al. 2019, Zheng et al. 2017</t>
   </si>
   <si>
     <t>HCA Immune 2018, Jaitin et al. 2019, Park et al. 2020, Zheng et al. 2017</t>
   </si>
   <si>
-    <t>CD79A, CD79B, CD19</t>
-  </si>
-  <si>
-    <t>FCER2, IGHD, CD22</t>
-  </si>
-  <si>
-    <t>POU2AF1, CD40, BIK</t>
+    <t>HCA Immune 2018, Jaitin et al. 2019, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, Jaitin et al. 2019, James et al. 2020</t>
+  </si>
+  <si>
+    <t>HCA Immune 2018, James et al. 2020, Li et al. 2019, Park et al. 2020</t>
+  </si>
+  <si>
+    <t>CD79A, MS4A1, CD19</t>
+  </si>
+  <si>
+    <t>CXCR5, TNFRSF13B, CD22</t>
+  </si>
+  <si>
+    <t>POU2AF1, CD40, SUGCT</t>
   </si>
   <si>
     <t>CR2, CD27, MS4A1</t>
   </si>
   <si>
-    <t>IGHM, MS4A1, TCL1A</t>
+    <t>IGHM, IGHD, TCL1A</t>
   </si>
   <si>
     <t>CD24, MYO1C, MS4A1</t>
@@ -1069,7 +1186,7 @@
     <t>CD22, ZCCHC7, CD24</t>
   </si>
   <si>
-    <t>CD22, EBF1, IGLL1</t>
+    <t>CD22, DNTT, IGLL1</t>
   </si>
   <si>
     <t>MKI67, TOP2A, CD19</t>
@@ -1090,31 +1207,31 @@
     <t>MKI67, TOP2A, CD3D</t>
   </si>
   <si>
-    <t>CD1C, FCER1A, ITGAX</t>
-  </si>
-  <si>
-    <t>BATF3, CADM1, RAB7B</t>
-  </si>
-  <si>
-    <t>CLEC10A, FCER1A, MSLN</t>
+    <t>CD1C, FCER1A, CLEC10A</t>
+  </si>
+  <si>
+    <t>BATF3, CADM1, CLEC9A</t>
+  </si>
+  <si>
+    <t>CLEC10A, FCER1A, CD1C</t>
   </si>
   <si>
     <t>CLEC10A, FCER1A, S100A9</t>
   </si>
   <si>
-    <t>EBI3, CCR7, FSCN1</t>
-  </si>
-  <si>
-    <t>CLEC10A, KLF4, RNF144B</t>
-  </si>
-  <si>
-    <t>ITGAX, CLEC10A, PCLAF</t>
+    <t>EBI3, CCR7, CCL19</t>
+  </si>
+  <si>
+    <t>CLEC10A, KLF4, AXL</t>
+  </si>
+  <si>
+    <t>IRF8, CLEC10A, PCLAF</t>
   </si>
   <si>
     <t>FXYD2, HES1, CD99</t>
   </si>
   <si>
-    <t>CD1A, CD1B, SMPD3</t>
+    <t>CD1A, CD8A, SMPD3</t>
   </si>
   <si>
     <t>PF4, CMTM5, SELP</t>
@@ -1129,10 +1246,10 @@
     <t>HBM, HBQ1, GYPA</t>
   </si>
   <si>
-    <t>CA1, KLF1, GATA2</t>
-  </si>
-  <si>
-    <t>GYPA, GYPB, SLC4A1</t>
+    <t>APOC1, KLF1, GATA2</t>
+  </si>
+  <si>
+    <t>GYPA, GYPB, HBA1</t>
   </si>
   <si>
     <t>KLF1, KCNH2, HBG1</t>
@@ -1147,7 +1264,7 @@
     <t>KIT, CPA3, SLC45A3</t>
   </si>
   <si>
-    <t>S100A8, S100A9, CTSG</t>
+    <t>S100A9, NAMPT, G0S2</t>
   </si>
   <si>
     <t>SPINK2, CTSG, FLT3</t>
@@ -1174,7 +1291,7 @@
     <t>SPINK2, MPO, CD34</t>
   </si>
   <si>
-    <t>KLRB1, TLE1, AREG</t>
+    <t>S100A13, TLE1, AREG</t>
   </si>
   <si>
     <t>CXCR3, CD3D, IKZF3</t>
@@ -1183,7 +1300,13 @@
     <t>GATA3, KLRG1, HPGDS</t>
   </si>
   <si>
-    <t>IL1R1, RORC, TOX</t>
+    <t>IL4I1, RORC, IL7R</t>
+  </si>
+  <si>
+    <t>GNLY, FCGR3A, NKG7</t>
+  </si>
+  <si>
+    <t>GNLY, CD160, NKG7</t>
   </si>
   <si>
     <t>GNLY, XCL2, NKG7</t>
@@ -1192,19 +1315,19 @@
     <t>CCL5, GZMK, FCGR3A</t>
   </si>
   <si>
-    <t>KLRB1, KIT, ZBTB16</t>
-  </si>
-  <si>
-    <t>LYVE1, KCNJ5, F13A1</t>
-  </si>
-  <si>
-    <t>SEPP1, CSF2RA, GPR34</t>
-  </si>
-  <si>
-    <t>CD5L, TIMD4, CETP</t>
-  </si>
-  <si>
-    <t>C1QA, CD68, APOE</t>
+    <t>LST1, KIT, SCN1B</t>
+  </si>
+  <si>
+    <t>LYVE1, SCIN, F13A1</t>
+  </si>
+  <si>
+    <t>SEPP1, CSF2RA, CD74</t>
+  </si>
+  <si>
+    <t>CD5L, VCAM1, CETP</t>
+  </si>
+  <si>
+    <t>C1QA, CD68, TREM2</t>
   </si>
   <si>
     <t>TPSAB1, TPSB2, CPA3</t>
@@ -1225,6 +1348,12 @@
     <t>LYZ, VCAN, S100A9</t>
   </si>
   <si>
+    <t>S100A9, CD14, S100A12</t>
+  </si>
+  <si>
+    <t>FCGR3A, C1QA, CX3CR1</t>
+  </si>
+  <si>
     <t>S100A9, LYZ, FCN1</t>
   </si>
   <si>
@@ -1237,10 +1366,10 @@
     <t>IL3RA, CCDC50, IRF7</t>
   </si>
   <si>
-    <t>JCHAIN, MZB1, DERL3</t>
-  </si>
-  <si>
-    <t>CSTA, RNASE2, LYZ</t>
+    <t>JCHAIN, MZB1, XBP1</t>
+  </si>
+  <si>
+    <t>CTSG, MPO, ELANE</t>
   </si>
   <si>
     <t>ZNF683, GNG4, PDCD1</t>
@@ -1249,46 +1378,46 @@
     <t>TOX2, SATB1, CCR9</t>
   </si>
   <si>
-    <t>GZMK, HLA-B, KLRK1</t>
-  </si>
-  <si>
-    <t>PDCD1, ICOS, LPAR6</t>
-  </si>
-  <si>
-    <t>TRDC, TRGC1, CCR9</t>
-  </si>
-  <si>
-    <t>IL7R, IL32, IFNG</t>
-  </si>
-  <si>
-    <t>KLRB1, SLC4A10, NCR3</t>
+    <t>NKG7, CD8A, CCL5</t>
+  </si>
+  <si>
+    <t>PDCD1, ICOS, CXCR5</t>
+  </si>
+  <si>
+    <t>TRDC, TRGC1, CCL5</t>
+  </si>
+  <si>
+    <t>IL7R, IL32, CD4</t>
+  </si>
+  <si>
+    <t>KLRB1, SLC4A10, TRAV1-2</t>
   </si>
   <si>
     <t>GZMK, CD4, IL10</t>
   </si>
   <si>
-    <t>GZMH, KLRD1, CD3G</t>
-  </si>
-  <si>
-    <t>CTLA4, CCR4, FOXP3</t>
-  </si>
-  <si>
-    <t>CD3D, CD3G, IL7R</t>
+    <t>NKG7, GNLY, CD8A</t>
+  </si>
+  <si>
+    <t>CTLA4, IL2RA, FOXP3</t>
+  </si>
+  <si>
+    <t>CD3D, CD3G, CD3E</t>
   </si>
   <si>
     <t>MIR155HG, BIRC3, SMS</t>
   </si>
   <si>
-    <t>CD8A, CCR7, CD7</t>
-  </si>
-  <si>
-    <t>CCR7, IL7R, CD4</t>
-  </si>
-  <si>
-    <t>GZMK, CD8A, IL32</t>
-  </si>
-  <si>
-    <t>IL32, IFITM1, CD4</t>
+    <t>CD8A, CCR7, SELL</t>
+  </si>
+  <si>
+    <t>CCR7, SELL, CD4</t>
+  </si>
+  <si>
+    <t>GZMK, CD8A, NKG7</t>
+  </si>
+  <si>
+    <t>IL32, SELL, CD4</t>
   </si>
   <si>
     <t>PDCD1, CD4, CTLA4</t>
@@ -1300,268 +1429,280 @@
     <t>CCL5, CXCR3, TBX21</t>
   </si>
   <si>
-    <t>IL7R, CCR6, KLRB1</t>
-  </si>
-  <si>
-    <t>HLA-DRB1, HLA-DPA1, TCL1A, MTRNR2L10, MS4A1, HLA-DRA, CD79B, CD74, CD79A, VPREB3</t>
-  </si>
-  <si>
-    <t>HLA-DRA, IGHD, CD83, MS4A1, IGHM, RNA18S5, CD79A, VPREB3, JCHAIN, IGHA1</t>
-  </si>
-  <si>
-    <t>IGKC, MYBL2, CD79B, TCL1A, CD19, MS4A1, SMIM14, POU2AF1, BIK, FCRLA</t>
-  </si>
-  <si>
-    <t>HLA-DPA1, TNFRSF13B, HLA-DRB1, HLA-DQA1, HLA-DPB1, IGKC, CD79A, HLA-DRA, MS4A1, CD74</t>
-  </si>
-  <si>
-    <t>HLA-DPB1, IGHD, CD74, MS4A1, HLA-DRA, HLA-DRB1, CD79A, IGHM, IGKC, TCL1A</t>
-  </si>
-  <si>
-    <t>LINC00926, MYO1C, CD79B, TCL1A, FAM129C, CD79A, IGHD, MS4A1, IGHM, VPREB3</t>
-  </si>
-  <si>
-    <t>VPREB1, CCDC191, ACSM3, FAM129C, PCDH9, CD24, VPREB3, IGHM, CD79B, TCL1A</t>
-  </si>
-  <si>
-    <t>RUBCNL, IGHM, GIHCG, CD79B, VPREB3, PCLAF, TCL1A, VPREB1, IGLL1, CD24</t>
-  </si>
-  <si>
-    <t>LAT2, CD79A, FAM129C, EBF1, ZCCHC7, VPREB1, VPREB3, IGLL1, CD79B, CD24</t>
-  </si>
-  <si>
-    <t>MME, AKAP12, CYGB, VPREB3, IGLL1, SOCS2, DNTT, FAM30A, CD79B, VPREB1</t>
-  </si>
-  <si>
-    <t>TCL1A, MYBL2, JCHAIN, SNX29P2, IGHA1, RNA18S5, LBHD1, RMI2, PCLAF, AC023590.1</t>
-  </si>
-  <si>
-    <t>FGL2, C1QC, FCGR2B, PTGS2, PKIB, DNASE1L3, IL1B, CLEC10A, SDS, P2RY6</t>
-  </si>
-  <si>
-    <t>KLRD1, KIFC1, GZMA, IFNG, NCR1, AURKB, SPC24, APOBEC3B, GPR174, KIR2DL4</t>
-  </si>
-  <si>
-    <t>C1QA, C1QC, PCLAF, HLA-DQB2, AC009501.4, SELENOP, IL1B, RNA18S5, DNASE1L3, ADAMDEC1</t>
-  </si>
-  <si>
-    <t>TYMS, TK1, EOMES, NKG7, CD160, CKS1B, KLRF1, CMC1, KLRD1, KIAA0101</t>
-  </si>
-  <si>
-    <t>PTTG1, CENPM, MIR4435-2HG, E2F1, BIRC5, TK1, LINC00152, CDKN3, KIAA0101, RRM2</t>
-  </si>
-  <si>
-    <t>HLA-DRA, CSF2RA, HLA-DRB5, HLA-DPB1, FCER1A, HLA-DPA1, HLA-DQA2, HLA-DQB1, HLA-DRB1, HLA-DQA1</t>
-  </si>
-  <si>
-    <t>HLA-DPB1, HLA-DQA1, HLA-DPA1, LGALS2, BATF3, SHTN1, WDFY4, CPVL, DNASE1L3, C1orf54</t>
-  </si>
-  <si>
-    <t>CD74, HLA-DQA1, HLA-DQB1, LYZ, CST3, HLA-DRB5, HLA-DPB1, HLA-DRB1, HLA-DPA1, HLA-DRA</t>
-  </si>
-  <si>
-    <t>CST3, RNASE2, S100A9, CLEC10A, FCER1A, LGALS2, CSTA, LYZ, FCN1, AC020656.1</t>
-  </si>
-  <si>
-    <t>CSF2RA, NCCRP1, MGLL, CCL19, RASSF4, EBI3, ARHGAP22, BCL2L14, LAD1, FSCN1</t>
-  </si>
-  <si>
-    <t>GGTA1P, CYP2S1, FTH1P10, ENHO, HLA-DPB2, RNF144B, CLEC10A, PPP1R14A, HLA-DRB6, NAPSB</t>
-  </si>
-  <si>
-    <t>HLA-DPA1, RNASE2, HLA-DPB1, HLA-DRA, LGALS1, LYZ, CST3, CLEC10A, PLD4, PCLAF</t>
-  </si>
-  <si>
-    <t>ID1, GNB2L1, DNTT, MZB1, SOX4, RP11-620J15.3, CD99, ADA, AC002454.1, PTCRA</t>
-  </si>
-  <si>
-    <t>SMPD3, MZB1, STMN1, CD1B, RP11-620J15.3, ATP5E, CD1E, ATP5L, GNB2L1, CD8B</t>
-  </si>
-  <si>
-    <t>GIHCG, PCLAF, IGSF10, CAVIN1, GMPR, MED12L, CMTM5, GATA2, ITGA2B, C2orf88</t>
-  </si>
-  <si>
-    <t>FABP4, PTRF, SPARCL1, CRIP2, CLDN5, PLVAP, ADIRF, CAV1, RAMP2, TM4SF1</t>
-  </si>
-  <si>
-    <t>DMKN, KRT15, KRT8, KRT17, CALML3, S100A14, CCL19, MDK, KRT5, KRT19</t>
-  </si>
-  <si>
-    <t>HBM, HBQ1, MYL4, KLF1, ALAS2, GYPB, GYPA, HBG2, RHAG, AHSP</t>
-  </si>
-  <si>
-    <t>FAM178B, PRSS57, HBB, HBD, AHSP, CA1, HBA1, GIHCG, KLF1, PCLAF</t>
-  </si>
-  <si>
-    <t>GYPA, HBG2, HBA2, HBA1, AHSP, GYPB, SLC4A1, ALAS2, HBG1, HBM</t>
-  </si>
-  <si>
-    <t>HBG1, CNRIP1, HBG2, HBA1, MYL4, HBA2, GIHCG, AHSP, FAM178B, KLF1</t>
-  </si>
-  <si>
-    <t>SMIM24, PRSS57, ACY3, CD34, SPINK2, KIAA0125, GUCY1A3, C1QTNF4, HOXA9, KCNK17</t>
-  </si>
-  <si>
-    <t>COL1A2, SEPP1, RARRES2, LUM, CALD1, COL3A1, FGF7, IGF2, COL1A1, DCN</t>
-  </si>
-  <si>
-    <t>CRYGD, CYTL1, SLC45A3, PRSS57, HPGDS, TPSB2, TPSAB1, CPA3, AL157895.1, GATA2</t>
-  </si>
-  <si>
-    <t>PRTN3, S100A8, PRSS57, MT-RNR2, MPO, AZU1, S100A9, CTSG, MT-RNR1, LYZ</t>
-  </si>
-  <si>
-    <t>NPR3, MPO, IGLL1, SMIM24, BAALC, GIHCG, PRSS57, FAM30A, SPINK2, C1QTNF4</t>
-  </si>
-  <si>
-    <t>TRGC1, HBA2, NBEAL1, HBA1, HBG2, ATP5MF, MICOS10, RIPOR2, ETS1, ATP5F1E</t>
-  </si>
-  <si>
-    <t>RUNX2, IGLL1, GIHCG, BAALC, C1QTNF4, SPINK2, FLT3, ACY3, AL096865.1, FAM30A</t>
-  </si>
-  <si>
-    <t>RNASE2, PRTN3, ELANE, NPW, AZU1, GIHCG, CTSG, C1QTNF4, MPO, PRSS57</t>
-  </si>
-  <si>
-    <t>HMGA2, CYTL1, CD34, PRSS57, SPINK2, EGFL7, GIHCG, ANKRD28, FAM30A, BEX3</t>
-  </si>
-  <si>
-    <t>HBD, FCER1A, NPR3, CKB, CYTL1, CNRIP1, CRYGD, PRSS57, GATA2, GIHCG</t>
-  </si>
-  <si>
-    <t>SNHG29, FCER1A, TFR2, CNRIP1, ITGA2B, CPA3, GATA2, CYTL1, PRSS57, GIHCG</t>
-  </si>
-  <si>
-    <t>SMIM24, PRTN3, MPO, RNASE2, GIHCG, AZU1, SPINK2, CLEC11A, PRSS57, PCLAF</t>
-  </si>
-  <si>
-    <t>KIT, MTRNR2L10, SPINK2, TNFRSF18, IGHA1, TLE1, IL4I1, KLRB1, KRT86, AREG</t>
-  </si>
-  <si>
-    <t>PFN1P1, TMSB10P1, MTRNR2L2, RPLP0P6, TMSB4XP8, RPL10P3, RPS3P6, RPL34P31, MTND4P12, MTCO3P12</t>
-  </si>
-  <si>
-    <t>C16orf54, TMSB4XP8, RPL10P3, MTND4P12, PFN1P1, RN7SL2, RNU1-1, SLITRK2, MTCO3P12, ADAM19</t>
-  </si>
-  <si>
-    <t>AHR, SPINK2, IL7R, KLRB1, IL4I1, KRT86, ENPP1, IL1R1, KIT, KRT81</t>
-  </si>
-  <si>
-    <t>TNFRSF18, XCL2, KLRD1, KLRC1, CMC1, GNLY, NKG7, CTSW, XCL1, KLRB1</t>
-  </si>
-  <si>
-    <t>GZMA, CD160, GZMB, GNLY, NKG7, CST7, HOPX, KLRF1, CMC1, KLRD1</t>
-  </si>
-  <si>
-    <t>LTB, KLRB1, KIT, BCAS1, IL1R1, AL450405.1, ZBTB16, IL4I1, SCN1B, HPN</t>
-  </si>
-  <si>
-    <t>SLC7A8, DAB2, OLFML2B, SIGLEC1, RIN2, F13A1, SLCO2B1, FP236383.3, STAB1, RNASE1</t>
-  </si>
-  <si>
-    <t>C1QB, C1QC, CD163, GPR34, FCGR2A, C1QA, VMO1, CSF2RA, VSIG4, SEPP1</t>
-  </si>
-  <si>
-    <t>CTSB, HMOX1, SELENOP, C1QA, LGMN, HBA2, HBA1, C1QB, HBG2, C1QC</t>
-  </si>
-  <si>
-    <t>NPC2, C1QA, HLA-DRA, SAT1, MS4A7, FCER1G, CST3, TYROBP, SEPP1, FTL</t>
-  </si>
-  <si>
-    <t>CNRIP1, CD9, VWA5A, KIT, TPSB2, HPGDS, GATA2, CPA3, LTC4S, TPSAB1</t>
-  </si>
-  <si>
-    <t>GATA2, CRYGD, CAVIN1, IGSF10, CYTL1, PRSS57, LINC02573, CRHBP, NPR3, GIHCG</t>
-  </si>
-  <si>
-    <t>C2orf88, CAVIN2, CLEC1B, NRGN, TUBB1, PPBP, CMTM5, GP9, PF4, ITGA2B</t>
-  </si>
-  <si>
-    <t>HLA-DPA1, FGL2, DNASE1L3, HLA-DQA1, IFI30, LGALS2, FAM26F, CLEC10A, MTRNR2L10, MTRNR2L8</t>
-  </si>
-  <si>
-    <t>NPC2, FTL, LST1, LGALS2, SAT1, TYROBP, FCER1G, GPX1, CST3, AIF1</t>
-  </si>
-  <si>
-    <t>TYROBP, CST3, FCN1, CSTA, LYZ, S100A9, S100A4, S100A6, S100A8, LGALS1</t>
-  </si>
-  <si>
-    <t>HLA-DRB5, FTL, LST1, NEAT1, CST3, SAT1, S100A8, S100A9, TYROBP, LYZ</t>
-  </si>
-  <si>
-    <t>S100A4, FTL, LGALS1, MIR1244-2, S100A6, MT-RNR2, S100A9, S100A8, LYZ, TYROBP</t>
-  </si>
-  <si>
-    <t>LILRA4, TPM2, JCHAIN, SPIB, UGCG, IRF8, CCDC50, IRF7, PLD4, TCF4</t>
-  </si>
-  <si>
-    <t>LINC00996, CCDC50, IRF7, SPIB, BLNK, PLD4, TNNI2, IL3RA, LILRA4, TPM2</t>
-  </si>
-  <si>
-    <t>IGHA2, TNFRSF17, IGHG3, IGHG1, IGHM, IGLC2, IGHA1, JCHAIN, IGKC, DERL3</t>
-  </si>
-  <si>
-    <t>LGALS1, RETN, FCN1, S100A8, AZU1, S100A9, AC020656.1, LYZ, RNASE2, CSTA</t>
-  </si>
-  <si>
-    <t>ATP5L, CD3D, GNB2L1, CD27, LEF1, ATP5E, TRAC, TRGC2, ZNF683, NUCB2</t>
-  </si>
-  <si>
-    <t>TOX2, ATP5L, ATP5E, CD3D, SATB1, ITM2A, TRAC, FYB, SOX4, GNB2L1</t>
-  </si>
-  <si>
-    <t>SNORA31, KRT13, GZMA, GZMK, CD8A, HLA-B, KLRK1, NKG7, AL450405.1, CCL5</t>
-  </si>
-  <si>
-    <t>CD40LG, RPL41, CD2, RPS29, KIAA1551, PDCD1, GIMAP7, GIMAP4, RPL17, TRAC</t>
-  </si>
-  <si>
-    <t>RTKN2, CCR9, CD7, TRGC1, LAYN, TRGC2, KLRC2, ITGA1, TRDC, KIR2DL4</t>
-  </si>
-  <si>
-    <t>RPL39, NBEAL1, LTB, JCHAIN, IL32, TRAC, RPS29, EEF1A1, RPL41, IGHA1</t>
-  </si>
-  <si>
-    <t>CCL5, GZMA, TRGC2, LYAR, NCR3, GZMK, KLRB1, LINC01871, SLC4A10, KLRG1</t>
-  </si>
-  <si>
-    <t>SELK, DUSP2, RGS1, DTHD1, IL10, GZMK, CTLA4, LINC00152, DUSP4, FAM46C</t>
-  </si>
-  <si>
-    <t>KLRD1, FGFBP2, IFNG, GZMH, NKG7, PRF1, CST7, KLRG1, AC092580.4, CCL5</t>
-  </si>
-  <si>
-    <t>LTB, B2M, TIGIT, LINC00152, IL32, HLA-A, DUSP4, S100A4, CTLA4, TRAC</t>
-  </si>
-  <si>
-    <t>TMEM66, SFTPA1, UQCR11.1, SCGB1A1, SCGB3A1, SCGB3A2, NBEAL1, RGS1, TRGC2, SFTPB</t>
-  </si>
-  <si>
-    <t>SOX4, MAGEH1, REL, TRAC, LAT, ATP5E, SATB1, ITM2A, C1orf228, GNB2L1</t>
-  </si>
-  <si>
-    <t>HSPH1, S100B, CD8B, CD3D, TRAC, IL32, LINC02446, CD8A, CD7, LTB</t>
-  </si>
-  <si>
-    <t>CHI3L2, IL32, OCIAD2, LTB, ITM2A, CRIP1, IFITM1, AC090498.1, RPL17, NBEAL1</t>
-  </si>
-  <si>
-    <t>CST7, C19orf43, GNB2L1, GZMK, B2M, ATP5L, CCL5, IL32, ATP5E, GLTSCR2</t>
-  </si>
-  <si>
-    <t>PTPRC, JUNB, RP11-290D2.6, CCR4, GPR183, AIM1, FAM46C, CTD-3252C9.4, LTB, IL32</t>
-  </si>
-  <si>
-    <t>ICA1, TMEM2, TIGIT, FAM46C, TOX2, PASK, ST8SIA1, CTLA4, PDCD1, ICOS</t>
-  </si>
-  <si>
-    <t>RGS1, EEF1A1, ATP5G2, TRAC, GLTSCR2, CD27, CCR7, FYB, GNB2L1, ATP5E</t>
-  </si>
-  <si>
-    <t>TNFAIP3, CD69, ANXA1, KLRB1, IGHA1, RPL17, FOSB, CCL5, GPR183, CRIP1</t>
-  </si>
-  <si>
-    <t>ANKRD28, CD69, TNFAIP3, ANXA1, ZBTB16, GPR183, RPL17, IL7R, KLRB1, RP11-356J5.12</t>
+    <t>IL7R, CCR6, ZBTB16</t>
+  </si>
+  <si>
+    <t>RACK1, HSPA1B, PTMA, HBG2, CD79A, HLA-DRB1, RPL10, MALAT1, ATP5F1E, HLA-DRA</t>
+  </si>
+  <si>
+    <t>MT-RNR2, RPL41, CD74, IGHA1, CXCR4, HLA-DRA, H3F3A, CD83, VPREB3, FTH1</t>
+  </si>
+  <si>
+    <t>KIAA0101, TCL1A, MS4A1, CELF2-AS2, RPS15A, OCM, FIGF, BCAN, AC245060.6, AL627171.2</t>
+  </si>
+  <si>
+    <t>HLA-DRA, MALAT1, MIR1244-2, RPS17, CD74, MT-ATP8, MT-ND4L, RPL39, HES1, RPL41</t>
+  </si>
+  <si>
+    <t>GNB2L1, IGHD, TCL1A, AL450405.1, YBX3, IGHM, CD74, PTPRC, ATP5E, IL4R</t>
+  </si>
+  <si>
+    <t>MIR1244-2, RPS24, CD79A, H3F3B, IGHM, TMSB10, PTMA, RPSAP15, ERICH5, RPL10P9</t>
+  </si>
+  <si>
+    <t>CD79B, PTMA, MIR1244-2, IGHM, CELF2-AS2, GBP7, AC020915.1, BCAN, SOX4, RPL21P134</t>
+  </si>
+  <si>
+    <t>IGLL1, TCL1A, PCLAF, VPREB1, PDLIM1, AC135507.1, RPSAP15, VAT1L, RP4-665J23.1, IER3-AS1</t>
+  </si>
+  <si>
+    <t>VPREB1, JCHAIN, IGLL1, LST1, RPSAP15, UHRF1, KIAA0226L, PTMA, RNU6-540P, MN1</t>
+  </si>
+  <si>
+    <t>DNTT, VPREB1, VPREB3, IGLL1, AC072061.1, RPSAP15, FTH1P20, AKAP12, AL021937.2, OR11G2</t>
+  </si>
+  <si>
+    <t>AC023590.1, RPSAP15, EFNB3, SAMMSON, DIO3OS, NDUFA6-DT, TCL1A, FTH1, RP11-736K20.5, RNU7-18P</t>
+  </si>
+  <si>
+    <t>RPSAP15, TMEM132C, MIR7111, SDS, AC005253.1, RNU6-151P, PRR16, AC107032.1, RNVU1-7, RPL7P52</t>
+  </si>
+  <si>
+    <t>RPSAP15, CELF2-AS2, HSPC324, TRBJ2-3, AL161781.2, OR11G2, AC004967.7, AC079610.2, PRR16, LINC00892</t>
+  </si>
+  <si>
+    <t>PCLAF, RPSAP15, AJ271736.10, MYOC, AP000936.1, AC107032.1, AL021937.2, TK1, AC090602.2, RNU6-540P</t>
+  </si>
+  <si>
+    <t>KIAA0101, STMN1, TUBA1B, TYMS, NKG7, ASPM, IGKC, HMGB2, HSPC324, CD38</t>
+  </si>
+  <si>
+    <t>STMN1, KIAA0101, IL32, ASPM, HMGB2, RRM2, RPSAP15, MT-CO3, TRBV28, SNORA67</t>
+  </si>
+  <si>
+    <t>RGS1, LYZ, HLA-DQA1, GPX1, HLA-DQB1, ENHO, CXCL10, FCER1A, CCL17, AL161781.2</t>
+  </si>
+  <si>
+    <t>C1orf54, LYZ, IRF8, RAB7B, WFDC21P, CPVL, RPSAP15, SNORA70, OR11G2, CHMP4BP1</t>
+  </si>
+  <si>
+    <t>RPL41, CLEC10A, JAML, H3F3A, RPL39, HLA-DQB1, EEF1A1, CST3, HLA-DRB5, HSPB1</t>
+  </si>
+  <si>
+    <t>LMNA, FCN1, RPSAP15, FMO2, PTMA, FCER1A, PRNCR1, POC1B-AS1, AC004967.7, SHISA3</t>
+  </si>
+  <si>
+    <t>NCCRP1, CCL19, TNFRSF11B, EBI3, RPSAP15, WNT5B, AC107032.1, RNU6-540P, SNORA70, HSPC324</t>
+  </si>
+  <si>
+    <t>PPM1J, HLA-DPB2, CXCL8, AXL, AL021937.2, PSMD6-AS1, RNU6-450P, SHISA3, RPSAP15, AL096870.2</t>
+  </si>
+  <si>
+    <t>PCLAF, CST3, RNASE2, RPSAP15, LY6E-DT, TRBV28, HLA-DRB6, TMSB10, LYZ, AL161781.2</t>
+  </si>
+  <si>
+    <t>CD99, PTCRA, IGLL1, FXYD2, MZB1, JCHAIN, RP11-620J15.3, PDLIM1, ADA, TMSB10</t>
+  </si>
+  <si>
+    <t>SMPD3, CD1B, SH3TC1, CD8B, CD1E, TCF7, TRDC, TRBC2, ELOVL4, CD8A</t>
+  </si>
+  <si>
+    <t>WFDC1, DNM3, GP1BA, MED12L, SLC18A2, SELP, RPSAP15, HSPC324, TBXA2R, OR11G2</t>
+  </si>
+  <si>
+    <t>ACKR1, RAMP3, PLVAP, CX3CL1, NRN1, SDPR, ZNF385D, MYRIP, HOXD8, TSPAN12</t>
+  </si>
+  <si>
+    <t>WFDC2, FRMD1, TOX3, FOXC1, CDH3, NXN, FAM150B, PNCK, IGDCC3, CDC42EP5</t>
+  </si>
+  <si>
+    <t>HBG2, RPSAP15, MYOC, PNMT, HBZ, FAM65C, AC004967.7, CH17-472G23.2, RPS2P44, SERPINB10</t>
+  </si>
+  <si>
+    <t>ERFE, FAM178B, HBB, RNF182, AFP, PCLAF, GAD1, AC106795.1, PRG2, RP4-717I23.3</t>
+  </si>
+  <si>
+    <t>RPSAP15, RP11-465B22.3, HMGCLL1, AL109767.1, AP000580.1, AL157938.1, HRCT1, CH17-472G23.2, HBA1, RP11-736K20.5</t>
+  </si>
+  <si>
+    <t>FAM178B, RPS4Y1, RPSAP15, PCLAF, SYNGR1, TMCC2, GIHCG, MAMLD1, BLVRB, AL592494.3</t>
+  </si>
+  <si>
+    <t>ACY3, SPINK2, KIAA0125, RP11-163E9.1, RPSAP15, AC096664.2, AC093635.1, INSL3, PRDM16, AC009041.2</t>
+  </si>
+  <si>
+    <t>NTRK2, SMOC2, SFRP1, OLFML1, PRRX1, SCARA5, RSPO3, ANGPTL1, NRK, ISLR</t>
+  </si>
+  <si>
+    <t>AL157895.1, MAMDC2, AC008781.2, AC026471.4, AL450384.2, AC004967.7, TPSB2, HSPC324, PAGE4, RPSAP15</t>
+  </si>
+  <si>
+    <t>PTPRC, LYZ, FTL, FTH1, S100A8, MT-RNR2, DEFA1, RPSAP15, MYOC, MT-RNR1</t>
+  </si>
+  <si>
+    <t>SPINK2, AC108866.1, LINC01786, RPL10P2, LINC01694, C1QTNF4, EEF1DP7, RPSAP15, AC092597.1, MIR4453HG</t>
+  </si>
+  <si>
+    <t>HBG2, HBA2, ATP5F1E, RACK1, IL32, HBA1, PTPRC, CST3, RPS17, H3F3A</t>
+  </si>
+  <si>
+    <t>AL096865.1, TRBV28, OSGEPL1-AS1, RNU6-450P, SPINK2, SSSCA1-AS1, RPSAP15, FAM30A, FALEC, ZNF280B</t>
+  </si>
+  <si>
+    <t>ELANE, SERPINB10, C1QTNF4, RPSAP15, HCG4P5, SNORA70, MPO, HOXA5, ZNF792, OR11G2</t>
+  </si>
+  <si>
+    <t>SPINK2, HOPX, RNU7-18P, MDK, LINC01011, AC007098.1, CD34, BEX3, AC007032.1, SERPINB10</t>
+  </si>
+  <si>
+    <t>GP9, CKB, FCER1A, PCLAF, CMTM5, RP11-357H14.17, CELF2-AS2, RP1-79C4.4, RPSAP15, AC107032.1</t>
+  </si>
+  <si>
+    <t>GIHCG, PRSS57, ITGA2B, CNRIP1, TPSAB1, EEF1A1P9, TMOD1, Z98884.1, AL691447.2, EML2-AS1</t>
+  </si>
+  <si>
+    <t>MPO, HIST1H1D, PRSS57, RPSAP15, PRTN3, RNU6-540P, AC104806.2, AL139246.3, AC009041.2, AC104563.1</t>
+  </si>
+  <si>
+    <t>AREG, IL7R, LST1, CSF2, TYROBP, MALAT1, S100A13, TNFSF13B, IGHA1, AC017002.1</t>
+  </si>
+  <si>
+    <t>RPS29P16, MTND4P12, RPS12P26, RPL23AP18, RPS3P6, RPL19P12, EIF1P3, RP4-665J23.1, MYOC, RPL37AP8</t>
+  </si>
+  <si>
+    <t>KRT1, MTCO3P12, MTND4P12, SLITRK2, RPSAP15, AC104563.1, TMEM132C, RPS2P44, CELF2-AS2, A2MP1</t>
+  </si>
+  <si>
+    <t>IL7R, TRDC, LINC00299, SLITRK2, TOX2, RPSAP15, CTSW, AC090948.3, XCL1, SPINK2</t>
+  </si>
+  <si>
+    <t>FCER1G, GNLY, TYROBP, IGFBP7, GZMB, MYOM2, PTGDS, LINC00299, FCGR3A, ADAMTS1</t>
+  </si>
+  <si>
+    <t>TYROBP, LDB2, CCL3, NKG7, FCER1G, GSTP1, KLRB1, CLIC3, IRF8, CXCL3</t>
+  </si>
+  <si>
+    <t>NKG7, CST3, GNLY, SPINK2, CDC20, RP11-445P19.3, HBG2, GPR56, IGFBP4, TTLL10</t>
+  </si>
+  <si>
+    <t>GNLY, TYROBP, IFITM2, H3F3B, CMC1, RPSAP15, MIR1244-2, KLRB1, STX17-AS1, MYOC</t>
+  </si>
+  <si>
+    <t>LST1, RBM24, HSPB1, NMU, HBA2, RPSAP15, AC016596.1, IL1A, RPS15A, CORO2B</t>
+  </si>
+  <si>
+    <t>PAGE4, CGA, LYVE1, METTL7B, SLC28A1, XAGE3, RPSAP15, AC090948.3, AC012085.2, AL513550.1</t>
+  </si>
+  <si>
+    <t>SEPP1, RPSAP15, RNU6-540P, AC007032.1, AL021937.2, AL592494.3, HMGCLL1, GATA6-AS1, ALOX15P1, LGR6</t>
+  </si>
+  <si>
+    <t>HBA2, CETP, HBG2, SNORD3D, TMSB10, HBA1, VCAM1, TMSB4X, EPB41L2, FTH1</t>
+  </si>
+  <si>
+    <t>GNLY, SEPP1, KIAA1598, IL8, CD5L, FTH1, FTL, AMICA1, APOE, C1QA</t>
+  </si>
+  <si>
+    <t>CPA3, TPSAB1, FTH1, PRG2, HPGDS, MYOC, RPSAP15, RP13-93L13.2, SLC18A2, RPS3AP12</t>
+  </si>
+  <si>
+    <t>FCER1A, VSTM1, LINC02573, HMGCLL1, AL356535.1, RNVU1-7, CYTL1, RPL19P12, TMEM132C, PRR16</t>
+  </si>
+  <si>
+    <t>RPSAP15, MYEOV, ESAM, OR11G2, HSPC324, AL021937.2, GPR150, RP13-93L13.2, C12orf42, CELF2-AS2</t>
+  </si>
+  <si>
+    <t>CST3, RPSAP15, FAM26F, CEBPD, IFI30, PTMA, MTRNR2L10, AC079610.2, SEPP1, MT-CO3</t>
+  </si>
+  <si>
+    <t>KLRB1, NKG7, C1QC, HLA-DRA, GPX1, FTH1, HBG2, SPRR3, KRT13, C1orf226</t>
+  </si>
+  <si>
+    <t>RETN, HBG2, LYZ, S100A8, FCN1, H3F3A, CRHR1-IT1, RPSAP15, RAB5IF, RP4-717I23.3</t>
+  </si>
+  <si>
+    <t>S100A9, ATP5E, FTL, NEAT1, TYROBP, HBG2, EEF1A1, CST3, MT-CO1, RPL7</t>
+  </si>
+  <si>
+    <t>RHOC, DNAJA4, HES4, HSPH1, HSPB1, MT2A, ABI3, CD52, MS4A7, ACTB</t>
+  </si>
+  <si>
+    <t>TYROBP, FTL, LYZ, NEAT1, HLA-DPB1, AL450405.1, AC090498.1, CYP4F3, AL355388.1, KIAA0101</t>
+  </si>
+  <si>
+    <t>FTH1, LYZ, FTL, S100A6, TYROBP, SRGN, PTPRC, MT-ND3, CROCC2, CST3</t>
+  </si>
+  <si>
+    <t>AL357143.1, PLD4, CACNB4, IRF8, GZMB, AC023590.1, JCHAIN, AC119428.2, AC098613.1, FTH1</t>
+  </si>
+  <si>
+    <t>TPM2, RPSAP15, TNNI2, IL3RA, SSTR3, RP4-665J23.1, PTPRR, LY6E-DT, AL161781.2, BTNL8</t>
+  </si>
+  <si>
+    <t>JCHAIN, MZB1, XBP1, HSP90B1, IGKC, IGHA2, TSPAN8, ITGA6-AS1, ELFN1-AS1, RPSAP15</t>
+  </si>
+  <si>
+    <t>PTMA, CFD, PCLAF, RP11-357H14.17, CLEC12B, LYZ, CITED1, SLC44A1, AC137630.3, RPSAP15</t>
+  </si>
+  <si>
+    <t>NUCB2, CD27, GAPDH, MALAT1, LEF1, VIM, CD8A, PRKCH, ZNF683, GNG4</t>
+  </si>
+  <si>
+    <t>MALAT1, ITM2A, CD1E, RPL10, SATB1, HSPH1, RPS27, FYB, FTL, TMSB10</t>
+  </si>
+  <si>
+    <t>CCL5, SERPINF1, CD8B, NKG7, CD8A, SOX4, KRT13, RP11-466H18.1, S100B, MT-RNR2</t>
+  </si>
+  <si>
+    <t>SOCS3, KLRB1, MALAT1, CH25H, PVALB, SRGN, ICOS, HMGCLL1, TRBV28, CELF2-AS2</t>
+  </si>
+  <si>
+    <t>KIR2DL4, KLRC2, LAYN, MYOC, IL1A, ASB15, SERPINB10, TRDC, LINC01635, DRAIC</t>
+  </si>
+  <si>
+    <t>RPL41, SYT14, GNB2L1, EEF1A1, GAS5, HLA-H, MT-RNR2, GLTSCR2, SPP1, RPS29</t>
+  </si>
+  <si>
+    <t>KLRB1, CEBPD, IL7R, GZMK, KLRG1, AC090498.1, RPS17, PRF1, SLC4A10, MT-ND3</t>
+  </si>
+  <si>
+    <t>GZMK, GZMA, DNTT, DONSON, RPSAP15, AL590822.2, YY2, AC007032.1, AC096733.2, MIR3188</t>
+  </si>
+  <si>
+    <t>NKG7, AIF1, GNLY, ITM2C, CD52, LDB2, HSPA1B, GZMH, PRDM16, RPL39</t>
+  </si>
+  <si>
+    <t>MS4A6A, IL32, TIMD4, SRGN, FTL, MIR3188, HLA-A, LINC00299, RTKN2, RPS27</t>
+  </si>
+  <si>
+    <t>RPS17, FCGR3A, MALAT1, RGS1, RPL39, SCGB3A2, KLRD1, TMEM66, CCL5, B2M</t>
+  </si>
+  <si>
+    <t>GAPDH, HLA-B, SMS, PKM, CD74, PTMA, TUBB, PTPRC, BIRC3, COTL1</t>
+  </si>
+  <si>
+    <t>CD8B, CD8A, RPS2, B2M, LINC02446, GNB2L1, HLA-B, HSPH1, RPL13, FTL</t>
+  </si>
+  <si>
+    <t>AL450405.1, MT-RNR2, EEF1A1, CTSL, IGLL5, TMSB10, FCGRT, RPS24, RPS18, GZMA</t>
+  </si>
+  <si>
+    <t>CCL5, GNB2L1, ATP5E, CD8B, HLA-B, TMEM66, CD1E, NKG7, RPL41, CD74</t>
+  </si>
+  <si>
+    <t>DNTT, MIR1244-2, GAS5, IL32, CD99, LTB, AC005912.1, NOP53, RPL34, SNHG29</t>
+  </si>
+  <si>
+    <t>SYN1, RNU6-540P, RP11-119D9.1, RPSAP15, PASK, HSPC324, AC010883.1, AC104563.1, AC096733.2, AP001059.3</t>
+  </si>
+  <si>
+    <t>GNB2L1, S100A4, HLA-B, RGS1, PTPRC, HLA-A, TSC22D3, GLTSCR2, SELM, RPS26</t>
+  </si>
+  <si>
+    <t>CCL5, KLRB1, DUSP2, GZMA, DNAJA4, RPL17, ANXA1, IGHA1, RPSAP15, DONSON</t>
+  </si>
+  <si>
+    <t>KLRB1, ANXA1, CEBPD, IL7R, IGHA1, ZNF683, RPLP1, RPSAP15, RPLP0, HLA-B</t>
   </si>
 </sst>
 </file>
@@ -1919,7 +2060,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H88"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1959,22 +2100,22 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E2" t="s">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="F2" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="G2" t="s">
-        <v>342</v>
+        <v>381</v>
       </c>
       <c r="H2" t="s">
-        <v>429</v>
+        <v>472</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -1985,22 +2126,22 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="E3" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="F3" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="G3" t="s">
-        <v>343</v>
+        <v>382</v>
       </c>
       <c r="H3" t="s">
-        <v>430</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -2011,22 +2152,22 @@
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="E4" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="F4" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="G4" t="s">
-        <v>344</v>
+        <v>383</v>
       </c>
       <c r="H4" t="s">
-        <v>431</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -2037,22 +2178,22 @@
         <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D5" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E5" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="F5" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="G5" t="s">
-        <v>345</v>
+        <v>384</v>
       </c>
       <c r="H5" t="s">
-        <v>432</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -2063,22 +2204,22 @@
         <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="E6" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="F6" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="G6" t="s">
-        <v>346</v>
+        <v>385</v>
       </c>
       <c r="H6" t="s">
-        <v>433</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -2089,22 +2230,22 @@
         <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
-        <v>190</v>
+        <v>198</v>
       </c>
       <c r="E7" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="F7" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G7" t="s">
-        <v>347</v>
+        <v>386</v>
       </c>
       <c r="H7" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -2115,22 +2256,22 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>191</v>
+        <v>199</v>
       </c>
       <c r="E8" t="s">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="F8" t="s">
-        <v>304</v>
+        <v>328</v>
       </c>
       <c r="G8" t="s">
-        <v>348</v>
+        <v>387</v>
       </c>
       <c r="H8" t="s">
-        <v>435</v>
+        <v>478</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -2141,22 +2282,22 @@
         <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="F9" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="G9" t="s">
-        <v>349</v>
+        <v>388</v>
       </c>
       <c r="H9" t="s">
-        <v>436</v>
+        <v>479</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -2167,22 +2308,22 @@
         <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>201</v>
       </c>
       <c r="E10" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="F10" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="G10" t="s">
-        <v>350</v>
+        <v>389</v>
       </c>
       <c r="H10" t="s">
-        <v>437</v>
+        <v>480</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -2193,22 +2334,22 @@
         <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
-        <v>194</v>
+        <v>202</v>
       </c>
       <c r="E11" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="F11" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="G11" t="s">
-        <v>351</v>
+        <v>390</v>
       </c>
       <c r="H11" t="s">
-        <v>438</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -2219,22 +2360,22 @@
         <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="E12" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="F12" t="s">
-        <v>300</v>
+        <v>330</v>
       </c>
       <c r="G12" t="s">
-        <v>352</v>
+        <v>391</v>
       </c>
       <c r="H12" t="s">
-        <v>439</v>
+        <v>482</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2245,22 +2386,22 @@
         <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="E13" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="F13" t="s">
-        <v>307</v>
+        <v>331</v>
       </c>
       <c r="G13" t="s">
-        <v>353</v>
+        <v>392</v>
       </c>
       <c r="H13" t="s">
-        <v>440</v>
+        <v>483</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -2271,22 +2412,22 @@
         <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="E14" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="F14" t="s">
-        <v>307</v>
+        <v>331</v>
       </c>
       <c r="G14" t="s">
-        <v>354</v>
+        <v>393</v>
       </c>
       <c r="H14" t="s">
-        <v>441</v>
+        <v>484</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -2297,22 +2438,22 @@
         <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E15" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
       <c r="F15" t="s">
-        <v>308</v>
+        <v>332</v>
       </c>
       <c r="G15" t="s">
-        <v>355</v>
+        <v>394</v>
       </c>
       <c r="H15" t="s">
-        <v>442</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -2323,22 +2464,22 @@
         <v>53</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D16" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="E16" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="F16" t="s">
-        <v>309</v>
+        <v>333</v>
       </c>
       <c r="G16" t="s">
-        <v>356</v>
+        <v>395</v>
       </c>
       <c r="H16" t="s">
-        <v>443</v>
+        <v>486</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2349,22 +2490,22 @@
         <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D17" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="E17" t="s">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="F17" t="s">
-        <v>301</v>
+        <v>334</v>
       </c>
       <c r="G17" t="s">
-        <v>357</v>
+        <v>396</v>
       </c>
       <c r="H17" t="s">
-        <v>444</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -2375,22 +2516,22 @@
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="E18" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="F18" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
       <c r="G18" t="s">
-        <v>358</v>
+        <v>397</v>
       </c>
       <c r="H18" t="s">
-        <v>445</v>
+        <v>488</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -2401,22 +2542,22 @@
         <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E19" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="F19" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="G19" t="s">
-        <v>359</v>
+        <v>398</v>
       </c>
       <c r="H19" t="s">
-        <v>446</v>
+        <v>489</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -2427,22 +2568,22 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="E20" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="F20" t="s">
-        <v>311</v>
+        <v>336</v>
       </c>
       <c r="G20" t="s">
-        <v>360</v>
+        <v>399</v>
       </c>
       <c r="H20" t="s">
-        <v>447</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -2453,22 +2594,22 @@
         <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D21" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="E21" t="s">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="F21" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G21" t="s">
-        <v>361</v>
+        <v>400</v>
       </c>
       <c r="H21" t="s">
-        <v>448</v>
+        <v>491</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -2479,22 +2620,22 @@
         <v>58</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D22" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="E22" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="F22" t="s">
-        <v>312</v>
+        <v>337</v>
       </c>
       <c r="G22" t="s">
-        <v>362</v>
+        <v>401</v>
       </c>
       <c r="H22" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -2505,22 +2646,22 @@
         <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D23" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E23" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="F23" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G23" t="s">
-        <v>363</v>
+        <v>402</v>
       </c>
       <c r="H23" t="s">
-        <v>450</v>
+        <v>493</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -2531,22 +2672,22 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="E24" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="F24" t="s">
-        <v>305</v>
+        <v>338</v>
       </c>
       <c r="G24" t="s">
-        <v>364</v>
+        <v>403</v>
       </c>
       <c r="H24" t="s">
-        <v>451</v>
+        <v>494</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -2557,22 +2698,22 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E25" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F25" t="s">
-        <v>313</v>
+        <v>339</v>
       </c>
       <c r="G25" t="s">
-        <v>365</v>
+        <v>404</v>
       </c>
       <c r="H25" t="s">
-        <v>452</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -2583,22 +2724,22 @@
         <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="D26" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="E26" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="F26" t="s">
-        <v>313</v>
+        <v>340</v>
       </c>
       <c r="G26" t="s">
-        <v>366</v>
+        <v>405</v>
       </c>
       <c r="H26" t="s">
-        <v>453</v>
+        <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -2609,22 +2750,22 @@
         <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E27" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="F27" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G27" t="s">
-        <v>367</v>
+        <v>406</v>
       </c>
       <c r="H27" t="s">
-        <v>454</v>
+        <v>497</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -2635,22 +2776,22 @@
         <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D28" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E28" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="F28" t="s">
-        <v>313</v>
+        <v>341</v>
       </c>
       <c r="G28" t="s">
-        <v>368</v>
+        <v>407</v>
       </c>
       <c r="H28" t="s">
-        <v>455</v>
+        <v>498</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -2661,22 +2802,22 @@
         <v>17</v>
       </c>
       <c r="C29" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D29" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="E29" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="F29" t="s">
-        <v>313</v>
+        <v>342</v>
       </c>
       <c r="G29" t="s">
-        <v>369</v>
+        <v>408</v>
       </c>
       <c r="H29" t="s">
-        <v>456</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -2687,22 +2828,22 @@
         <v>18</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="D30" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E30" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="F30" t="s">
-        <v>314</v>
+        <v>343</v>
       </c>
       <c r="G30" t="s">
-        <v>370</v>
+        <v>409</v>
       </c>
       <c r="H30" t="s">
-        <v>457</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -2713,22 +2854,22 @@
         <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D31" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E31" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
       <c r="F31" t="s">
-        <v>305</v>
+        <v>338</v>
       </c>
       <c r="G31" t="s">
-        <v>371</v>
+        <v>410</v>
       </c>
       <c r="H31" t="s">
-        <v>458</v>
+        <v>501</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -2739,22 +2880,22 @@
         <v>61</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D32" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E32" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="F32" t="s">
-        <v>305</v>
+        <v>344</v>
       </c>
       <c r="G32" t="s">
-        <v>372</v>
+        <v>411</v>
       </c>
       <c r="H32" t="s">
-        <v>459</v>
+        <v>502</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2765,22 +2906,22 @@
         <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E33" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="F33" t="s">
-        <v>305</v>
+        <v>344</v>
       </c>
       <c r="G33" t="s">
-        <v>373</v>
+        <v>412</v>
       </c>
       <c r="H33" t="s">
-        <v>460</v>
+        <v>503</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2791,22 +2932,22 @@
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="E34" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F34" t="s">
-        <v>313</v>
+        <v>339</v>
       </c>
       <c r="G34" t="s">
-        <v>374</v>
+        <v>413</v>
       </c>
       <c r="H34" t="s">
-        <v>461</v>
+        <v>504</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2817,22 +2958,22 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D35" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="E35" t="s">
-        <v>267</v>
+        <v>278</v>
       </c>
       <c r="F35" t="s">
-        <v>313</v>
+        <v>340</v>
       </c>
       <c r="G35" t="s">
-        <v>375</v>
+        <v>414</v>
       </c>
       <c r="H35" t="s">
-        <v>462</v>
+        <v>505</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2843,22 +2984,22 @@
         <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D36" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="E36" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="F36" t="s">
-        <v>315</v>
+        <v>345</v>
       </c>
       <c r="G36" t="s">
-        <v>376</v>
+        <v>415</v>
       </c>
       <c r="H36" t="s">
-        <v>463</v>
+        <v>506</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2869,22 +3010,22 @@
         <v>63</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="E37" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
       <c r="F37" t="s">
-        <v>316</v>
+        <v>346</v>
       </c>
       <c r="G37" t="s">
-        <v>377</v>
+        <v>416</v>
       </c>
       <c r="H37" t="s">
-        <v>464</v>
+        <v>507</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2895,22 +3036,22 @@
         <v>64</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="E38" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="F38" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G38" t="s">
-        <v>378</v>
+        <v>417</v>
       </c>
       <c r="H38" t="s">
-        <v>465</v>
+        <v>508</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2921,22 +3062,22 @@
         <v>65</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D39" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E39" t="s">
-        <v>272</v>
+        <v>285</v>
       </c>
       <c r="F39" t="s">
-        <v>317</v>
+        <v>347</v>
       </c>
       <c r="G39" t="s">
-        <v>379</v>
+        <v>418</v>
       </c>
       <c r="H39" t="s">
-        <v>466</v>
+        <v>509</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -2947,22 +3088,22 @@
         <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E40" t="s">
-        <v>256</v>
+        <v>286</v>
       </c>
       <c r="F40" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G40" t="s">
-        <v>380</v>
+        <v>419</v>
       </c>
       <c r="H40" t="s">
-        <v>467</v>
+        <v>510</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2973,22 +3114,22 @@
         <v>67</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D41" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="E41" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="F41" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G41" t="s">
-        <v>381</v>
+        <v>420</v>
       </c>
       <c r="H41" t="s">
-        <v>468</v>
+        <v>511</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2999,22 +3140,22 @@
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="E42" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="F42" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="G42" t="s">
-        <v>382</v>
+        <v>421</v>
       </c>
       <c r="H42" t="s">
-        <v>469</v>
+        <v>512</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -3025,22 +3166,22 @@
         <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D43" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E43" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="F43" t="s">
-        <v>317</v>
+        <v>348</v>
       </c>
       <c r="G43" t="s">
-        <v>383</v>
+        <v>422</v>
       </c>
       <c r="H43" t="s">
-        <v>470</v>
+        <v>513</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -3051,22 +3192,22 @@
         <v>69</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D44" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E44" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="F44" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="G44" t="s">
-        <v>384</v>
+        <v>423</v>
       </c>
       <c r="H44" t="s">
-        <v>471</v>
+        <v>514</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -3077,22 +3218,22 @@
         <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D45" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="E45" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="F45" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="G45" t="s">
-        <v>385</v>
+        <v>424</v>
       </c>
       <c r="H45" t="s">
-        <v>472</v>
+        <v>515</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -3103,22 +3244,22 @@
         <v>24</v>
       </c>
       <c r="C46" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="E46" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="F46" t="s">
-        <v>318</v>
+        <v>349</v>
       </c>
       <c r="G46" t="s">
-        <v>386</v>
+        <v>425</v>
       </c>
       <c r="H46" t="s">
-        <v>473</v>
+        <v>516</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -3129,22 +3270,22 @@
         <v>71</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D47" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="E47" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="F47" t="s">
-        <v>319</v>
+        <v>350</v>
       </c>
       <c r="G47" t="s">
-        <v>387</v>
+        <v>426</v>
       </c>
       <c r="H47" t="s">
-        <v>474</v>
+        <v>517</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -3155,22 +3296,22 @@
         <v>72</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E48" t="s">
-        <v>274</v>
+        <v>290</v>
       </c>
       <c r="F48" t="s">
-        <v>319</v>
+        <v>351</v>
       </c>
       <c r="G48" t="s">
-        <v>388</v>
+        <v>427</v>
       </c>
       <c r="H48" t="s">
-        <v>475</v>
+        <v>518</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -3181,22 +3322,22 @@
         <v>73</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D49" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="E49" t="s">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="F49" t="s">
-        <v>320</v>
+        <v>352</v>
       </c>
       <c r="G49" t="s">
-        <v>389</v>
+        <v>428</v>
       </c>
       <c r="H49" t="s">
-        <v>476</v>
+        <v>519</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -3207,22 +3348,22 @@
         <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D50" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="E50" t="s">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="F50" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="G50" t="s">
-        <v>390</v>
+        <v>429</v>
       </c>
       <c r="H50" t="s">
-        <v>477</v>
+        <v>520</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -3233,100 +3374,100 @@
         <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>224</v>
+        <v>206</v>
       </c>
       <c r="E51" t="s">
-        <v>256</v>
+        <v>293</v>
       </c>
       <c r="F51" t="s">
-        <v>304</v>
+        <v>354</v>
       </c>
       <c r="G51" t="s">
-        <v>391</v>
+        <v>430</v>
       </c>
       <c r="H51" t="s">
-        <v>478</v>
+        <v>521</v>
       </c>
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
       <c r="E52" t="s">
-        <v>269</v>
+        <v>293</v>
       </c>
       <c r="F52" t="s">
-        <v>305</v>
+        <v>354</v>
       </c>
       <c r="G52" t="s">
-        <v>392</v>
+        <v>431</v>
       </c>
       <c r="H52" t="s">
-        <v>479</v>
+        <v>522</v>
       </c>
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="E53" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="F53" t="s">
-        <v>315</v>
+        <v>355</v>
       </c>
       <c r="G53" t="s">
-        <v>393</v>
+        <v>432</v>
       </c>
       <c r="H53" t="s">
-        <v>480</v>
+        <v>523</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D54" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="E54" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="F54" t="s">
-        <v>322</v>
+        <v>348</v>
       </c>
       <c r="G54" t="s">
-        <v>394</v>
+        <v>433</v>
       </c>
       <c r="H54" t="s">
-        <v>481</v>
+        <v>524</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -3337,22 +3478,22 @@
         <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D55" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="E55" t="s">
-        <v>272</v>
+        <v>295</v>
       </c>
       <c r="F55" t="s">
-        <v>317</v>
+        <v>345</v>
       </c>
       <c r="G55" t="s">
-        <v>395</v>
+        <v>434</v>
       </c>
       <c r="H55" t="s">
-        <v>482</v>
+        <v>525</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -3360,441 +3501,441 @@
         <v>26</v>
       </c>
       <c r="B56" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D56" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="E56" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="F56" t="s">
-        <v>323</v>
+        <v>356</v>
       </c>
       <c r="G56" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
       <c r="H56" t="s">
-        <v>483</v>
+        <v>526</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B57" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C57" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="E57" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="F57" t="s">
-        <v>324</v>
+        <v>348</v>
       </c>
       <c r="G57" t="s">
-        <v>397</v>
+        <v>436</v>
       </c>
       <c r="H57" t="s">
-        <v>484</v>
+        <v>527</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B58" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D58" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="E58" t="s">
-        <v>256</v>
+        <v>297</v>
       </c>
       <c r="F58" t="s">
-        <v>304</v>
+        <v>357</v>
       </c>
       <c r="G58" t="s">
-        <v>398</v>
+        <v>437</v>
       </c>
       <c r="H58" t="s">
-        <v>485</v>
+        <v>528</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D59" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="E59" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="F59" t="s">
-        <v>325</v>
+        <v>358</v>
       </c>
       <c r="G59" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
       <c r="H59" t="s">
-        <v>486</v>
+        <v>529</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C60" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D60" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="E60" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="F60" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G60" t="s">
-        <v>400</v>
+        <v>439</v>
       </c>
       <c r="H60" t="s">
-        <v>487</v>
+        <v>530</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B61" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D61" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="E61" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F61" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G61" t="s">
-        <v>401</v>
+        <v>440</v>
       </c>
       <c r="H61" t="s">
-        <v>488</v>
+        <v>531</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B62" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D62" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
       <c r="E62" t="s">
-        <v>260</v>
+        <v>299</v>
       </c>
       <c r="F62" t="s">
-        <v>305</v>
+        <v>359</v>
       </c>
       <c r="G62" t="s">
-        <v>402</v>
+        <v>441</v>
       </c>
       <c r="H62" t="s">
-        <v>489</v>
+        <v>532</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B63" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C63" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D63" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
       <c r="E63" t="s">
-        <v>284</v>
+        <v>300</v>
       </c>
       <c r="F63" t="s">
-        <v>328</v>
+        <v>360</v>
       </c>
       <c r="G63" t="s">
-        <v>403</v>
+        <v>442</v>
       </c>
       <c r="H63" t="s">
-        <v>490</v>
+        <v>533</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B64" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C64" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="D64" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="E64" t="s">
-        <v>257</v>
+        <v>287</v>
       </c>
       <c r="F64" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="G64" t="s">
-        <v>404</v>
+        <v>443</v>
       </c>
       <c r="H64" t="s">
-        <v>491</v>
+        <v>534</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B65" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C65" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D65" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="E65" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="F65" t="s">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c r="G65" t="s">
-        <v>405</v>
+        <v>444</v>
       </c>
       <c r="H65" t="s">
-        <v>492</v>
+        <v>535</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B66" t="s">
-        <v>36</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D66" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="E66" t="s">
-        <v>272</v>
+        <v>302</v>
       </c>
       <c r="F66" t="s">
-        <v>317</v>
+        <v>361</v>
       </c>
       <c r="G66" t="s">
-        <v>406</v>
+        <v>445</v>
       </c>
       <c r="H66" t="s">
-        <v>493</v>
+        <v>536</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="D67" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="E67" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="F67" t="s">
-        <v>330</v>
+        <v>362</v>
       </c>
       <c r="G67" t="s">
-        <v>407</v>
+        <v>446</v>
       </c>
       <c r="H67" t="s">
-        <v>494</v>
+        <v>537</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B68" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C68" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D68" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="E68" t="s">
-        <v>256</v>
+        <v>294</v>
       </c>
       <c r="F68" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="G68" t="s">
-        <v>408</v>
+        <v>447</v>
       </c>
       <c r="H68" t="s">
-        <v>495</v>
+        <v>538</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B69" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="C69" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="D69" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
       <c r="E69" t="s">
-        <v>267</v>
+        <v>303</v>
       </c>
       <c r="F69" t="s">
-        <v>313</v>
+        <v>363</v>
       </c>
       <c r="G69" t="s">
-        <v>409</v>
+        <v>448</v>
       </c>
       <c r="H69" t="s">
-        <v>496</v>
+        <v>539</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B70" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="D70" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="E70" t="s">
-        <v>267</v>
+        <v>287</v>
       </c>
       <c r="F70" t="s">
-        <v>313</v>
+        <v>348</v>
       </c>
       <c r="G70" t="s">
-        <v>410</v>
+        <v>449</v>
       </c>
       <c r="H70" t="s">
-        <v>497</v>
+        <v>540</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
-        <v>81</v>
+        <v>37</v>
       </c>
       <c r="C71" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D71" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="E71" t="s">
-        <v>287</v>
+        <v>304</v>
       </c>
       <c r="F71" t="s">
-        <v>331</v>
+        <v>364</v>
       </c>
       <c r="G71" t="s">
-        <v>411</v>
+        <v>450</v>
       </c>
       <c r="H71" t="s">
-        <v>498</v>
+        <v>541</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B72" t="s">
-        <v>82</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D72" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="E72" t="s">
-        <v>288</v>
+        <v>266</v>
       </c>
       <c r="F72" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G72" t="s">
-        <v>412</v>
+        <v>451</v>
       </c>
       <c r="H72" t="s">
-        <v>499</v>
+        <v>542</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3805,22 +3946,22 @@
         <v>83</v>
       </c>
       <c r="C73" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D73" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="E73" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="F73" t="s">
-        <v>333</v>
+        <v>365</v>
       </c>
       <c r="G73" t="s">
-        <v>413</v>
+        <v>452</v>
       </c>
       <c r="H73" t="s">
-        <v>500</v>
+        <v>543</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3831,22 +3972,22 @@
         <v>84</v>
       </c>
       <c r="C74" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D74" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="E74" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="F74" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="G74" t="s">
-        <v>414</v>
+        <v>453</v>
       </c>
       <c r="H74" t="s">
-        <v>501</v>
+        <v>544</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3857,22 +3998,22 @@
         <v>85</v>
       </c>
       <c r="C75" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="E75" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="F75" t="s">
-        <v>315</v>
+        <v>366</v>
       </c>
       <c r="G75" t="s">
-        <v>415</v>
+        <v>454</v>
       </c>
       <c r="H75" t="s">
-        <v>502</v>
+        <v>545</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3883,22 +4024,22 @@
         <v>86</v>
       </c>
       <c r="C76" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D76" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="E76" t="s">
-        <v>267</v>
+        <v>307</v>
       </c>
       <c r="F76" t="s">
-        <v>313</v>
+        <v>367</v>
       </c>
       <c r="G76" t="s">
-        <v>416</v>
+        <v>455</v>
       </c>
       <c r="H76" t="s">
-        <v>503</v>
+        <v>546</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3909,22 +4050,22 @@
         <v>87</v>
       </c>
       <c r="C77" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D77" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="E77" t="s">
-        <v>292</v>
+        <v>308</v>
       </c>
       <c r="F77" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="G77" t="s">
-        <v>417</v>
+        <v>456</v>
       </c>
       <c r="H77" t="s">
-        <v>504</v>
+        <v>547</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3935,22 +4076,22 @@
         <v>88</v>
       </c>
       <c r="C78" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D78" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="E78" t="s">
-        <v>293</v>
+        <v>309</v>
       </c>
       <c r="F78" t="s">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c r="G78" t="s">
-        <v>418</v>
+        <v>457</v>
       </c>
       <c r="H78" t="s">
-        <v>505</v>
+        <v>548</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3958,25 +4099,25 @@
         <v>39</v>
       </c>
       <c r="B79" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C79" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D79" t="s">
-        <v>199</v>
+        <v>251</v>
       </c>
       <c r="E79" t="s">
-        <v>294</v>
+        <v>310</v>
       </c>
       <c r="F79" t="s">
-        <v>337</v>
+        <v>369</v>
       </c>
       <c r="G79" t="s">
-        <v>419</v>
+        <v>458</v>
       </c>
       <c r="H79" t="s">
-        <v>506</v>
+        <v>549</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3984,25 +4125,25 @@
         <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C80" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="D80" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="E80" t="s">
-        <v>267</v>
+        <v>277</v>
       </c>
       <c r="F80" t="s">
-        <v>313</v>
+        <v>339</v>
       </c>
       <c r="G80" t="s">
-        <v>420</v>
+        <v>459</v>
       </c>
       <c r="H80" t="s">
-        <v>507</v>
+        <v>550</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -4010,25 +4151,25 @@
         <v>39</v>
       </c>
       <c r="B81" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C81" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D81" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="E81" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
       <c r="F81" t="s">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c r="G81" t="s">
-        <v>421</v>
+        <v>460</v>
       </c>
       <c r="H81" t="s">
-        <v>508</v>
+        <v>551</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -4036,25 +4177,25 @@
         <v>39</v>
       </c>
       <c r="B82" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C82" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D82" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="E82" t="s">
-        <v>296</v>
+        <v>312</v>
       </c>
       <c r="F82" t="s">
-        <v>339</v>
+        <v>371</v>
       </c>
       <c r="G82" t="s">
-        <v>422</v>
+        <v>461</v>
       </c>
       <c r="H82" t="s">
-        <v>509</v>
+        <v>552</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -4062,25 +4203,25 @@
         <v>39</v>
       </c>
       <c r="B83" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
       <c r="C83" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D83" t="s">
-        <v>247</v>
+        <v>207</v>
       </c>
       <c r="E83" t="s">
-        <v>297</v>
+        <v>313</v>
       </c>
       <c r="F83" t="s">
-        <v>340</v>
+        <v>372</v>
       </c>
       <c r="G83" t="s">
-        <v>423</v>
+        <v>462</v>
       </c>
       <c r="H83" t="s">
-        <v>510</v>
+        <v>553</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -4091,22 +4232,22 @@
         <v>93</v>
       </c>
       <c r="C84" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D84" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="E84" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="F84" t="s">
-        <v>341</v>
+        <v>373</v>
       </c>
       <c r="G84" t="s">
-        <v>424</v>
+        <v>463</v>
       </c>
       <c r="H84" t="s">
-        <v>511</v>
+        <v>554</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -4117,22 +4258,22 @@
         <v>94</v>
       </c>
       <c r="C85" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="D85" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="E85" t="s">
-        <v>267</v>
+        <v>315</v>
       </c>
       <c r="F85" t="s">
-        <v>313</v>
+        <v>374</v>
       </c>
       <c r="G85" t="s">
-        <v>425</v>
+        <v>464</v>
       </c>
       <c r="H85" t="s">
-        <v>512</v>
+        <v>555</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -4143,22 +4284,22 @@
         <v>95</v>
       </c>
       <c r="C86" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D86" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="E86" t="s">
-        <v>267</v>
+        <v>316</v>
       </c>
       <c r="F86" t="s">
-        <v>313</v>
+        <v>375</v>
       </c>
       <c r="G86" t="s">
-        <v>426</v>
+        <v>465</v>
       </c>
       <c r="H86" t="s">
-        <v>513</v>
+        <v>556</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -4169,22 +4310,22 @@
         <v>96</v>
       </c>
       <c r="C87" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="D87" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="E87" t="s">
-        <v>252</v>
+        <v>317</v>
       </c>
       <c r="F87" t="s">
-        <v>307</v>
+        <v>376</v>
       </c>
       <c r="G87" t="s">
-        <v>427</v>
+        <v>466</v>
       </c>
       <c r="H87" t="s">
-        <v>514</v>
+        <v>557</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -4195,22 +4336,126 @@
         <v>97</v>
       </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="D88" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="E88" t="s">
-        <v>289</v>
+        <v>318</v>
       </c>
       <c r="F88" t="s">
-        <v>333</v>
+        <v>377</v>
       </c>
       <c r="G88" t="s">
-        <v>428</v>
+        <v>467</v>
       </c>
       <c r="H88" t="s">
-        <v>515</v>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8">
+      <c r="A89" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" t="s">
+        <v>98</v>
+      </c>
+      <c r="C89" t="s">
+        <v>189</v>
+      </c>
+      <c r="D89" t="s">
+        <v>258</v>
+      </c>
+      <c r="E89" t="s">
+        <v>277</v>
+      </c>
+      <c r="F89" t="s">
+        <v>339</v>
+      </c>
+      <c r="G89" t="s">
+        <v>468</v>
+      </c>
+      <c r="H89" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8">
+      <c r="A90" t="s">
+        <v>39</v>
+      </c>
+      <c r="B90" t="s">
+        <v>99</v>
+      </c>
+      <c r="C90" t="s">
+        <v>190</v>
+      </c>
+      <c r="D90" t="s">
+        <v>254</v>
+      </c>
+      <c r="E90" t="s">
+        <v>319</v>
+      </c>
+      <c r="F90" t="s">
+        <v>378</v>
+      </c>
+      <c r="G90" t="s">
+        <v>469</v>
+      </c>
+      <c r="H90" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8">
+      <c r="A91" t="s">
+        <v>39</v>
+      </c>
+      <c r="B91" t="s">
+        <v>100</v>
+      </c>
+      <c r="C91" t="s">
+        <v>191</v>
+      </c>
+      <c r="D91" t="s">
+        <v>259</v>
+      </c>
+      <c r="E91" t="s">
+        <v>320</v>
+      </c>
+      <c r="F91" t="s">
+        <v>379</v>
+      </c>
+      <c r="G91" t="s">
+        <v>470</v>
+      </c>
+      <c r="H91" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8">
+      <c r="A92" t="s">
+        <v>39</v>
+      </c>
+      <c r="B92" t="s">
+        <v>101</v>
+      </c>
+      <c r="C92" t="s">
+        <v>192</v>
+      </c>
+      <c r="D92" t="s">
+        <v>260</v>
+      </c>
+      <c r="E92" t="s">
+        <v>321</v>
+      </c>
+      <c r="F92" t="s">
+        <v>380</v>
+      </c>
+      <c r="G92" t="s">
+        <v>471</v>
+      </c>
+      <c r="H92" t="s">
+        <v>562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>